<commit_message>
detalles finales de despliegue
</commit_message>
<xml_diff>
--- a/salidas/importances.xlsx
+++ b/salidas/importances.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>importances</t>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Importance</t>
         </is>
       </c>
     </row>
@@ -444,7 +449,12 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>0.1614879943239598</v>
       </c>
     </row>
@@ -452,7 +462,12 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DistanceFromHome</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>0.1281821614991341</v>
       </c>
     </row>
@@ -460,7 +475,12 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>EnvironmentSatisfaction</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>0.07404096898397018</v>
       </c>
     </row>
@@ -468,7 +488,12 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>JobSatisfaction</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>0.05876414509458821</v>
       </c>
     </row>
@@ -476,7 +501,12 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MonthlyIncome</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>0.2210644516318866</v>
       </c>
     </row>
@@ -484,7 +514,12 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NumCompaniesWorked</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>0.08308063915303025</v>
       </c>
     </row>
@@ -492,7 +527,12 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TotalWorkingYears</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>0.1358501379999026</v>
       </c>
     </row>
@@ -500,7 +540,12 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>YearsSinceLastPromotion</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>0.06314551812069231</v>
       </c>
     </row>
@@ -508,7 +553,12 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>YearsWithCurrManager</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>0.07438398319283601</v>
       </c>
     </row>

</xml_diff>